<commit_message>
maj manifeste et ressources
</commit_message>
<xml_diff>
--- a/tipote-knowledge/manifest/resources_manifest.xlsx
+++ b/tipote-knowledge/manifest/resources_manifest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
   <si>
     <t>id</t>
   </si>
@@ -243,6 +243,81 @@
   </si>
   <si>
     <t>Trouver des idées de thèmes de newsletters intéressantes pour les inscrits d'une liste emails</t>
+  </si>
+  <si>
+    <t>guide_lead_magnets</t>
+  </si>
+  <si>
+    <t>Guide complet pour créer des lead magnets</t>
+  </si>
+  <si>
+    <t>guides/guide-complet-lead-magnets.docx</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>lead_magnet</t>
+  </si>
+  <si>
+    <t>créer_lead_magnet</t>
+  </si>
+  <si>
+    <t>Trouver et créer un bon lead magnet selon son activité et le promouvoir efficacement  pour capturer des emails qualifiés</t>
+  </si>
+  <si>
+    <t>50_idees_lead_magnets</t>
+  </si>
+  <si>
+    <t>50 Idées de Lead Magnets</t>
+  </si>
+  <si>
+    <t>swipefiles/liste-idees-lead-magnets.docx</t>
+  </si>
+  <si>
+    <t>idées_lead_magnet</t>
+  </si>
+  <si>
+    <t>Trouver une bonne idée de lead magnet pour attirer les bons prospects</t>
+  </si>
+  <si>
+    <t>trouver_clients_reseaux_sociaux</t>
+  </si>
+  <si>
+    <t>Trouver des clients sur les réseaux sociaux</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>notes/trouver_des_clients_reseaux_sociaux.txt</t>
+  </si>
+  <si>
+    <t>réseaux_sociaux</t>
+  </si>
+  <si>
+    <t>trouver_clients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quelques insights pour trouver des clients sur les réseaux sociaux en infiltrant des groupes </t>
+  </si>
+  <si>
+    <t>astuces_promotion_lead_magnet</t>
+  </si>
+  <si>
+    <t>23 astuces redoutables pour promouvoir ton lead magnet</t>
+  </si>
+  <si>
+    <t>guide/astuces-promouvoir-lead-magnet.docx</t>
+  </si>
+  <si>
+    <t>promouvoir_lead_magnet</t>
+  </si>
+  <si>
+    <t>Astuces pour promouvoir son lead magnet et trouver des prospects de qualité</t>
   </si>
 </sst>
 </file>
@@ -1101,18 +1176,38 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="A11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="K11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1129,18 +1224,38 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="A12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="K12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1157,18 +1272,38 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="K13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1185,18 +1320,38 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="K14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>

</xml_diff>